<commit_message>
Correção da base final
</commit_message>
<xml_diff>
--- a/Docs/Dicionario de Dados.xlsx
+++ b/Docs/Dicionario de Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP ProBook 640\Desktop\TCC\MPAlugueisLisboa\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\johns\Desktop\TCC\MPAlugueisLisboa\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC5B1D0-EB4E-4A10-91ED-AE1835754286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B452B8E-3D07-4211-A524-3DBCB3BC43EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47970B15-0966-45D8-8208-C78DF7F64898}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{47970B15-0966-45D8-8208-C78DF7F64898}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="267">
   <si>
     <t>Localização do Imovel</t>
   </si>
@@ -508,22 +508,335 @@
   </si>
   <si>
     <t>VARIAVEL</t>
+  </si>
+  <si>
+    <t>Ambito Geografico</t>
+  </si>
+  <si>
+    <t>Regiao</t>
+  </si>
+  <si>
+    <t>Cidades</t>
+  </si>
+  <si>
+    <t>qtd Idade 0 -14</t>
+  </si>
+  <si>
+    <t>qtd Idade 15-64</t>
+  </si>
+  <si>
+    <t>qtd idade &gt;65</t>
+  </si>
+  <si>
+    <t>% Idade 0 -14</t>
+  </si>
+  <si>
+    <t>% Idade 15-64</t>
+  </si>
+  <si>
+    <t>% idade &gt;65</t>
+  </si>
+  <si>
+    <t>% cidadÃ£os estrangeiros,em relacao total da populaÃ§Ã£o</t>
+  </si>
+  <si>
+    <t>qtd Hospitais particulares e publicos</t>
+  </si>
+  <si>
+    <t>qtd Farmacias</t>
+  </si>
+  <si>
+    <t>Quantidade construÃ§oes novas</t>
+  </si>
+  <si>
+    <t>qtd escolas - pre-escolar -4 -6 anos</t>
+  </si>
+  <si>
+    <t>qtd escolas - ciclo 1 - 6-10 anos</t>
+  </si>
+  <si>
+    <t>qtd escolas - ciclo 2 - 10 -12 anos</t>
+  </si>
+  <si>
+    <t>qtd escolas - ciclo 3 - 13 -15 anos</t>
+  </si>
+  <si>
+    <t>qtd shows,exibicoes,teatro</t>
+  </si>
+  <si>
+    <t>qtd Cinemas</t>
+  </si>
+  <si>
+    <t>Ganho medio mensal</t>
+  </si>
+  <si>
+    <t>% Desempregados</t>
+  </si>
+  <si>
+    <t>% Poder de compra</t>
+  </si>
+  <si>
+    <t>% Crimes</t>
+  </si>
+  <si>
+    <t>qtd bancos</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>distance_driving_Lisboa_Portugal</t>
+  </si>
+  <si>
+    <t>distance_driving_Porto_Portugal</t>
+  </si>
+  <si>
+    <t>Clima_Ranking</t>
+  </si>
+  <si>
+    <t>Ranking_Geral</t>
+  </si>
+  <si>
+    <t>Ranking_Regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N.Âº mÃ©dio de indivÃ­duos por KmÂ²	</t>
+  </si>
+  <si>
+    <t>Região</t>
+  </si>
+  <si>
+    <t>Âmbito Geográfico: indica a região geográfica do município.</t>
+  </si>
+  <si>
+    <t>Âmbito Geográfico: indica o nome da cidade.</t>
+  </si>
+  <si>
+    <t>Quantidade Idade 0-14</t>
+  </si>
+  <si>
+    <t>Quantidade de Indivíduos com Idade de 0 a 14 anos.</t>
+  </si>
+  <si>
+    <t>Quantidade Idade 15-64</t>
+  </si>
+  <si>
+    <t>Quantidade de Indivíduos com Idade de 15 a 64 anos.</t>
+  </si>
+  <si>
+    <t>Quantidade Idade &gt;65</t>
+  </si>
+  <si>
+    <t>Quantidade de Indivíduos com Idade acima de 65 anos.</t>
+  </si>
+  <si>
+    <t>Percentual Idade 0-14</t>
+  </si>
+  <si>
+    <t>Percentual de Indivíduos com Idade de 0 a 14 anos.</t>
+  </si>
+  <si>
+    <t>Percentual Idade 15-64</t>
+  </si>
+  <si>
+    <t>Percentual de Indivíduos com Idade de 15 a 64 anos.</t>
+  </si>
+  <si>
+    <t>Percentual Idade &gt;65</t>
+  </si>
+  <si>
+    <t>Percentual de Indivíduos com Idade acima de 65 anos.</t>
+  </si>
+  <si>
+    <t>N.º médio de indivíduos por Km²</t>
+  </si>
+  <si>
+    <t>Número médio de indivíduos por quilômetro quadrado.</t>
+  </si>
+  <si>
+    <t>Percentual Cidadãos Estrangeiros</t>
+  </si>
+  <si>
+    <t>Percentual de Cidadãos Estrangeiros em relação à população total.</t>
+  </si>
+  <si>
+    <t>Quantidade Hospitais (Particulares e Público</t>
+  </si>
+  <si>
+    <t>s) Quantidade de Hospitais Particulares e Públicos.</t>
+  </si>
+  <si>
+    <t>Quantidade Farmácias</t>
+  </si>
+  <si>
+    <t>Quantidade de Farmácias.</t>
+  </si>
+  <si>
+    <t>Quantidade Construções Novas</t>
+  </si>
+  <si>
+    <t>Quantidade de Construções Novas.</t>
+  </si>
+  <si>
+    <t>Quantidade Escolas Pré-Escolar (4-6 anos)</t>
+  </si>
+  <si>
+    <t>Quantidade de Escolas de Pré-Escolar (4 a 6 anos).</t>
+  </si>
+  <si>
+    <t>Quantidade Escolas Ciclo 1 (6-10 anos)</t>
+  </si>
+  <si>
+    <t>Quantidade de Escolas do Ciclo 1 (6 a 10 anos).</t>
+  </si>
+  <si>
+    <t>Quantidade Escolas Ciclo 2 (10-12 anos)</t>
+  </si>
+  <si>
+    <t>Quantidade de Escolas do Ciclo 2 (10 a 12 anos).</t>
+  </si>
+  <si>
+    <t>Quantidade Escolas Ciclo 3 (13-15 anos)</t>
+  </si>
+  <si>
+    <t>Quantidade de Escolas do Ciclo 3 (13 a 15 anos).</t>
+  </si>
+  <si>
+    <t>Quantidade Shows, Exibições, Teatro</t>
+  </si>
+  <si>
+    <t>Quantidade de Shows, Exibições e Teatros.</t>
+  </si>
+  <si>
+    <t>Quantidade Cinemas</t>
+  </si>
+  <si>
+    <t>Quantidade de Cinemas.</t>
+  </si>
+  <si>
+    <t>Ganho Médio Mensal</t>
+  </si>
+  <si>
+    <t>Ganho Médio Mensal.</t>
+  </si>
+  <si>
+    <t>Percentual Desempregados</t>
+  </si>
+  <si>
+    <t>Percentual de Desempregados.</t>
+  </si>
+  <si>
+    <t>Percentual Poder de Compra</t>
+  </si>
+  <si>
+    <t>Percentual de Poder de Compra.</t>
+  </si>
+  <si>
+    <t>Percentual Crimes</t>
+  </si>
+  <si>
+    <t>Percentual de Crimes.</t>
+  </si>
+  <si>
+    <t>Quantidade de Bancos.</t>
+  </si>
+  <si>
+    <t>Latitude: indica a latitude geográfica do município.</t>
+  </si>
+  <si>
+    <t>Longitude: indica a longitude geográfica do município.</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>Endereço: contém o endereço completo do imóvel, incluindo rua, número, cidade, estado e código postal.</t>
+  </si>
+  <si>
+    <t>Distância (dirigindo) de Lisboa, Portugal</t>
+  </si>
+  <si>
+    <t>Distância (em condução) entre o município e Lisboa, Portugal.</t>
+  </si>
+  <si>
+    <t>Distância (dirigindo) do Porto, Portugal</t>
+  </si>
+  <si>
+    <t>Distância (em condução) entre o município e Porto, Portugal.</t>
+  </si>
+  <si>
+    <t>Ranking Clima</t>
+  </si>
+  <si>
+    <t>Ranking do Clima.</t>
+  </si>
+  <si>
+    <t>Ranking Geral</t>
+  </si>
+  <si>
+    <t>Ranking Geral do município.</t>
+  </si>
+  <si>
+    <t>Ranking Regional</t>
+  </si>
+  <si>
+    <t>Ranking Regional do município.</t>
+  </si>
+  <si>
+    <t>Quantidade Bancos</t>
+  </si>
+  <si>
+    <t>Nivel geografico</t>
+  </si>
+  <si>
+    <t>MUNICIPIOS</t>
+  </si>
+  <si>
+    <t>Distribuiçao Faixa Etaria</t>
+  </si>
+  <si>
+    <t>densidade populacional</t>
+  </si>
+  <si>
+    <t>Serviços de Saude</t>
+  </si>
+  <si>
+    <t>Desenvolvimento urbano</t>
+  </si>
+  <si>
+    <t>Educação</t>
+  </si>
+  <si>
+    <t>Cultura e Lazer</t>
+  </si>
+  <si>
+    <t>Emprego e Renda</t>
+  </si>
+  <si>
+    <t>Segurança</t>
+  </si>
+  <si>
+    <t>Localização Municipio</t>
+  </si>
+  <si>
+    <t>Distancia Liboa</t>
+  </si>
+  <si>
+    <t>Distancia Porto</t>
+  </si>
+  <si>
+    <t>Ranaking Regional</t>
+  </si>
+  <si>
+    <t>NOME LOGICO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -551,10 +864,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,7 +1183,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91833DD-397B-4478-A1CF-EE89DDD9277B}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -877,9 +1191,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" customWidth="1"/>
+    <col min="13" max="13" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +1210,7 @@
         <v>159</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>266</v>
       </c>
       <c r="E1" t="s">
         <v>81</v>
@@ -1144,7 +1461,7 @@
       <c r="B16" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>30</v>
       </c>
       <c r="D16" t="s">
@@ -1766,8 +2083,566 @@
         <v>144</v>
       </c>
     </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>253</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>160</v>
+      </c>
+      <c r="D53" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" t="s">
+        <v>252</v>
+      </c>
+    </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
+      <c r="A54" t="s">
+        <v>253</v>
+      </c>
+      <c r="B54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>161</v>
+      </c>
+      <c r="D54" t="s">
+        <v>191</v>
+      </c>
+      <c r="E54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>253</v>
+      </c>
+      <c r="B55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" t="s">
+        <v>162</v>
+      </c>
+      <c r="E55" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>253</v>
+      </c>
+      <c r="B56" t="s">
+        <v>254</v>
+      </c>
+      <c r="C56" t="s">
+        <v>163</v>
+      </c>
+      <c r="D56" t="s">
+        <v>194</v>
+      </c>
+      <c r="E56" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>253</v>
+      </c>
+      <c r="B57" t="s">
+        <v>254</v>
+      </c>
+      <c r="C57" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" t="s">
+        <v>196</v>
+      </c>
+      <c r="E57" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>253</v>
+      </c>
+      <c r="B58" t="s">
+        <v>254</v>
+      </c>
+      <c r="C58" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" t="s">
+        <v>198</v>
+      </c>
+      <c r="E58" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>253</v>
+      </c>
+      <c r="B59" t="s">
+        <v>254</v>
+      </c>
+      <c r="C59" t="s">
+        <v>166</v>
+      </c>
+      <c r="D59" t="s">
+        <v>200</v>
+      </c>
+      <c r="E59" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>253</v>
+      </c>
+      <c r="B60" t="s">
+        <v>254</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" t="s">
+        <v>202</v>
+      </c>
+      <c r="E60" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>253</v>
+      </c>
+      <c r="B61" t="s">
+        <v>254</v>
+      </c>
+      <c r="C61" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" t="s">
+        <v>204</v>
+      </c>
+      <c r="E61" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>253</v>
+      </c>
+      <c r="B62" t="s">
+        <v>255</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" t="s">
+        <v>206</v>
+      </c>
+      <c r="E62" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>253</v>
+      </c>
+      <c r="B63" t="s">
+        <v>255</v>
+      </c>
+      <c r="C63" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" t="s">
+        <v>208</v>
+      </c>
+      <c r="E63" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>253</v>
+      </c>
+      <c r="B64" t="s">
+        <v>256</v>
+      </c>
+      <c r="C64" t="s">
+        <v>170</v>
+      </c>
+      <c r="D64" t="s">
+        <v>210</v>
+      </c>
+      <c r="E64" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>253</v>
+      </c>
+      <c r="B65" t="s">
+        <v>256</v>
+      </c>
+      <c r="C65" t="s">
+        <v>171</v>
+      </c>
+      <c r="D65" t="s">
+        <v>212</v>
+      </c>
+      <c r="E65" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>253</v>
+      </c>
+      <c r="B66" t="s">
+        <v>257</v>
+      </c>
+      <c r="C66" t="s">
+        <v>172</v>
+      </c>
+      <c r="D66" t="s">
+        <v>214</v>
+      </c>
+      <c r="E66" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>253</v>
+      </c>
+      <c r="B67" t="s">
+        <v>258</v>
+      </c>
+      <c r="C67" t="s">
+        <v>173</v>
+      </c>
+      <c r="D67" t="s">
+        <v>216</v>
+      </c>
+      <c r="E67" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>253</v>
+      </c>
+      <c r="B68" t="s">
+        <v>258</v>
+      </c>
+      <c r="C68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" t="s">
+        <v>218</v>
+      </c>
+      <c r="E68" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>253</v>
+      </c>
+      <c r="B69" t="s">
+        <v>258</v>
+      </c>
+      <c r="C69" t="s">
+        <v>175</v>
+      </c>
+      <c r="D69" t="s">
+        <v>220</v>
+      </c>
+      <c r="E69" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>253</v>
+      </c>
+      <c r="B70" t="s">
+        <v>258</v>
+      </c>
+      <c r="C70" t="s">
+        <v>176</v>
+      </c>
+      <c r="D70" t="s">
+        <v>222</v>
+      </c>
+      <c r="E70" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>253</v>
+      </c>
+      <c r="B71" t="s">
+        <v>259</v>
+      </c>
+      <c r="C71" t="s">
+        <v>177</v>
+      </c>
+      <c r="D71" t="s">
+        <v>224</v>
+      </c>
+      <c r="E71" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>253</v>
+      </c>
+      <c r="B72" t="s">
+        <v>259</v>
+      </c>
+      <c r="C72" t="s">
+        <v>178</v>
+      </c>
+      <c r="D72" t="s">
+        <v>226</v>
+      </c>
+      <c r="E72" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>253</v>
+      </c>
+      <c r="B73" t="s">
+        <v>260</v>
+      </c>
+      <c r="C73" t="s">
+        <v>179</v>
+      </c>
+      <c r="D73" t="s">
+        <v>228</v>
+      </c>
+      <c r="E73" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>253</v>
+      </c>
+      <c r="B74" t="s">
+        <v>260</v>
+      </c>
+      <c r="C74" t="s">
+        <v>180</v>
+      </c>
+      <c r="D74" t="s">
+        <v>230</v>
+      </c>
+      <c r="E74" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>253</v>
+      </c>
+      <c r="B75" t="s">
+        <v>260</v>
+      </c>
+      <c r="C75" t="s">
+        <v>181</v>
+      </c>
+      <c r="D75" t="s">
+        <v>232</v>
+      </c>
+      <c r="E75" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>253</v>
+      </c>
+      <c r="B76" t="s">
+        <v>261</v>
+      </c>
+      <c r="C76" t="s">
+        <v>182</v>
+      </c>
+      <c r="D76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E76" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>253</v>
+      </c>
+      <c r="B77" t="s">
+        <v>257</v>
+      </c>
+      <c r="C77" t="s">
+        <v>183</v>
+      </c>
+      <c r="D77" t="s">
+        <v>251</v>
+      </c>
+      <c r="E77" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>253</v>
+      </c>
+      <c r="B78" t="s">
+        <v>262</v>
+      </c>
+      <c r="C78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>253</v>
+      </c>
+      <c r="B79" t="s">
+        <v>262</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>253</v>
+      </c>
+      <c r="B80" t="s">
+        <v>262</v>
+      </c>
+      <c r="C80" t="s">
+        <v>184</v>
+      </c>
+      <c r="D80" t="s">
+        <v>239</v>
+      </c>
+      <c r="E80" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>253</v>
+      </c>
+      <c r="B81" t="s">
+        <v>263</v>
+      </c>
+      <c r="C81" t="s">
+        <v>185</v>
+      </c>
+      <c r="D81" t="s">
+        <v>241</v>
+      </c>
+      <c r="E81" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>253</v>
+      </c>
+      <c r="B82" t="s">
+        <v>264</v>
+      </c>
+      <c r="C82" t="s">
+        <v>186</v>
+      </c>
+      <c r="D82" t="s">
+        <v>243</v>
+      </c>
+      <c r="E82" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>253</v>
+      </c>
+      <c r="B83" t="s">
+        <v>245</v>
+      </c>
+      <c r="C83" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" t="s">
+        <v>245</v>
+      </c>
+      <c r="E83" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>253</v>
+      </c>
+      <c r="B84" t="s">
+        <v>247</v>
+      </c>
+      <c r="C84" t="s">
+        <v>188</v>
+      </c>
+      <c r="D84" t="s">
+        <v>247</v>
+      </c>
+      <c r="E84" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>253</v>
+      </c>
+      <c r="B85" t="s">
+        <v>265</v>
+      </c>
+      <c r="C85" t="s">
+        <v>189</v>
+      </c>
+      <c r="D85" t="s">
+        <v>249</v>
+      </c>
+      <c r="E85" t="s">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E52" xr:uid="{F91833DD-397B-4478-A1CF-EE89DDD9277B}"/>

</xml_diff>